<commit_message>
Commit some mixed layer depth estimates from PAL1314 CTD casts
</commit_message>
<xml_diff>
--- a/data/raw/PAL1314_LMG1401_PAL_LTER_data/Selected CTD - PAL-LTER 2013-2014.xlsx
+++ b/data/raw/PAL1314_LMG1401_PAL_LTER_data/Selected CTD - PAL-LTER 2013-2014.xlsx
@@ -1,29 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcollins/Code/LipidPhotoOxBox/data/raw/PAL1314_LMG1401_PAL_LTER_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesrco/Code/LipidPhotoOxBox/data/raw/PAL1314_LMG1401_PAL_LTER_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="PAL-LTER B 20131231" sheetId="6" r:id="rId1"/>
-    <sheet name="PAL-LTER B 20131227" sheetId="5" r:id="rId2"/>
-    <sheet name="PAL-LTER E 20131227" sheetId="4" r:id="rId3"/>
-    <sheet name="PAL-LTER B 20131224" sheetId="3" r:id="rId4"/>
-    <sheet name="PAL-LTER B 20131212" sheetId="2" r:id="rId5"/>
+    <sheet name="PAL-LTER E 20140102" sheetId="8" r:id="rId1"/>
+    <sheet name="PAL-LTER B 20140102" sheetId="7" r:id="rId2"/>
+    <sheet name="PAL-LTER B 20131231" sheetId="6" r:id="rId3"/>
+    <sheet name="PAL-LTER B 20131227" sheetId="5" r:id="rId4"/>
+    <sheet name="PAL-LTER E 20131227" sheetId="4" r:id="rId5"/>
+    <sheet name="PAL-LTER B 20131224" sheetId="3" r:id="rId6"/>
+    <sheet name="PAL-LTER B 20131212" sheetId="2" r:id="rId7"/>
+    <sheet name="MLD Calculations" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="s2013346a.s87" localSheetId="4">'PAL-LTER B 20131212'!$A$1:$C$57</definedName>
-    <definedName name="s2013358a.s87" localSheetId="3">'PAL-LTER B 20131224'!$A$1:$C$56</definedName>
-    <definedName name="s2013361a.s87" localSheetId="2">'PAL-LTER E 20131227'!$A$1:$C$32</definedName>
-    <definedName name="s2013361b.s87" localSheetId="1">'PAL-LTER B 20131227'!$A$1:$C$56</definedName>
-    <definedName name="s2013365a.s87" localSheetId="0">'PAL-LTER B 20131231'!$A$1:$C$62</definedName>
+    <definedName name="s2013346a.s87" localSheetId="6">'PAL-LTER B 20131212'!$A$1:$C$57</definedName>
+    <definedName name="s2013358a.s87" localSheetId="5">'PAL-LTER B 20131224'!$A$1:$C$56</definedName>
+    <definedName name="s2013361a.s87" localSheetId="4">'PAL-LTER E 20131227'!$A$1:$C$32</definedName>
+    <definedName name="s2013361b.s87" localSheetId="3">'PAL-LTER B 20131227'!$A$1:$C$56</definedName>
+    <definedName name="s2013365a.s87" localSheetId="2">'PAL-LTER B 20131231'!$A$1:$C$62</definedName>
+    <definedName name="s2014002a.s87" localSheetId="0">'PAL-LTER E 20140102'!$A$1:$C$71</definedName>
+    <definedName name="s2014002b.s87" localSheetId="1">'PAL-LTER B 20140102'!$A$1:$C$56</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -40,7 +45,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="s2013346a.s87" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013346a.s87.txt">
+    <textPr fileType="mac" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013346a.s87.txt">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -49,7 +54,7 @@
     </textPr>
   </connection>
   <connection id="2" name="s2013358a.s87" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013358a.s87.txt">
+    <textPr fileType="mac" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013358a.s87.txt">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -58,7 +63,7 @@
     </textPr>
   </connection>
   <connection id="3" name="s2013361a.s87" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013361a.s87.txt">
+    <textPr fileType="mac" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013361a.s87.txt">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -67,7 +72,7 @@
     </textPr>
   </connection>
   <connection id="4" name="s2013361b.s87" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013361b.s87.txt">
+    <textPr fileType="mac" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013361b.s87.txt">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -75,8 +80,26 @@
     </textPr>
   </connection>
   <connection id="5" name="s2013365a.s87" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013365a.s87.txt">
+    <textPr fileType="mac" sourceFile="/Users/jrcollins/Downloads/1314pal/ctd/s87/s2013365a.s87.txt">
       <textFields count="2">
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="s2014002a.s87" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/jamesrco/Downloads/1314pal/ctd/s87/s2014002a.s87.txt">
+      <textFields count="3">
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" name="s2014002b.s87" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="/Users/jamesrco/Downloads/1314pal/ctd/s87/s2014002b.s87.txt">
+      <textFields count="3">
+        <textField/>
         <textField/>
         <textField/>
       </textFields>
@@ -86,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>C328L -0999  001 -64.7800 -64.0810 2013/12/12 346 10:01  LTERpal1314</t>
   </si>
@@ -135,15 +158,70 @@
   <si>
     <t>$ 21-Nov-2014 R.Iannuzzi lter2s87.m 58.0 maxPress s2013365a.std</t>
   </si>
+  <si>
+    <t>C328L -0999  001 -64.8140 -64.0420 2014/01/02   2 09:59  LTERpal1314</t>
+  </si>
+  <si>
+    <t>$ LTER event 39 at 621.167 35.957 Palmer Station E (pal1314)</t>
+  </si>
+  <si>
+    <t>$ 21-Nov-2014 R.Iannuzzi lter2s87.m 67.0 maxPress s2014002a.std</t>
+  </si>
+  <si>
+    <t>C328L -0999  001 -64.7800 -64.0810 2014/01/02   2 10:59  LTERpal1314</t>
+  </si>
+  <si>
+    <t>$ LTER event 39 at 622.804 39.852 Palmer Station B (pal1314)</t>
+  </si>
+  <si>
+    <t>$ 21-Nov-2014 R.Iannuzzi lter2s87.m 52.0 maxPress s2014002b.std</t>
+  </si>
+  <si>
+    <t>PAL1314 calculations of mixed later depth</t>
+  </si>
+  <si>
+    <t>Using criteria of Levitus (1982); MLD = depth at which the temperature difference from the surface is 0.5 deg C</t>
+  </si>
+  <si>
+    <t>Station.Name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>MLD.depth.m</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,13 +244,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -186,22 +269,30 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="s2014002a.s87" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="s2014002b.s87" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="s2013365a.s87" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="s2013361b.s87" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="s2013361a.s87" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="s2013358a.s87" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="s2013346a.s87" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -468,9 +559,1614 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D71"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="C5">
+        <v>33.387</v>
+      </c>
+      <c r="D5">
+        <f>B5-$B$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="C6">
+        <v>33.430999999999997</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D35" si="0">B6-$B$5</f>
+        <v>-0.1180000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="C7">
+        <v>33.472999999999999</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-0.16400000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="C8">
+        <v>33.47</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-0.19600000000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="C9">
+        <v>33.491999999999997</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-0.23700000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="C10">
+        <v>33.517000000000003</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-0.26900000000000007</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="C11">
+        <v>33.536999999999999</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-0.28500000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="C12">
+        <v>33.555999999999997</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-0.29400000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>0.38</v>
+      </c>
+      <c r="C13">
+        <v>33.56</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-0.30100000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="C14">
+        <v>33.564</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-0.31400000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="C15">
+        <v>33.58</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-0.34500000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="C16">
+        <v>33.603000000000002</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-0.38200000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="C17">
+        <v>33.624000000000002</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-0.40800000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>0.253</v>
+      </c>
+      <c r="C18">
+        <v>33.646999999999998</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-0.42800000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="C19">
+        <v>33.68</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-0.44800000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>0.224</v>
+      </c>
+      <c r="C20">
+        <v>33.716999999999999</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>-0.45700000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>0.214</v>
+      </c>
+      <c r="C21">
+        <v>33.749000000000002</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-0.46700000000000008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="C22">
+        <v>33.779000000000003</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-0.47900000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>0.184</v>
+      </c>
+      <c r="C23">
+        <v>33.802</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>-0.49700000000000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>0.159</v>
+      </c>
+      <c r="C24">
+        <v>33.823999999999998</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-0.52200000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="C25">
+        <v>33.845999999999997</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>-0.54900000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>0.115</v>
+      </c>
+      <c r="C26">
+        <v>33.862000000000002</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-0.56600000000000006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>0.106</v>
+      </c>
+      <c r="C27">
+        <v>33.874000000000002</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>-0.57500000000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="C28">
+        <v>33.884999999999998</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-0.58500000000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="C29">
+        <v>33.890999999999998</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>-0.59400000000000008</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C30">
+        <v>33.893999999999998</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-0.59800000000000009</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="C31">
+        <v>33.898000000000003</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>-0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="C32">
+        <v>33.901000000000003</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>-0.60200000000000009</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C33">
+        <v>33.906999999999996</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>-0.6080000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="C34">
+        <v>33.921999999999997</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>-0.6140000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="C35">
+        <v>33.941000000000003</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>-0.62200000000000011</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C36">
+        <v>33.959000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>-3.0000000000000001E-3</v>
+      </c>
+      <c r="C37">
+        <v>33.970999999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>-6.2E-2</v>
+      </c>
+      <c r="C38">
+        <v>33.984000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>-0.156</v>
+      </c>
+      <c r="C39">
+        <v>33.997999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>-0.246</v>
+      </c>
+      <c r="C40">
+        <v>34.012999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>-0.34</v>
+      </c>
+      <c r="C41">
+        <v>34.021999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>-0.40400000000000003</v>
+      </c>
+      <c r="C42">
+        <v>34.026000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>-0.40400000000000003</v>
+      </c>
+      <c r="C43">
+        <v>34.043999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>-0.375</v>
+      </c>
+      <c r="C44">
+        <v>34.061999999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>-0.35799999999999998</v>
+      </c>
+      <c r="C45">
+        <v>34.067999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>-0.35299999999999998</v>
+      </c>
+      <c r="C46">
+        <v>34.070999999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <v>-0.35</v>
+      </c>
+      <c r="C47">
+        <v>34.070999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>-0.34699999999999998</v>
+      </c>
+      <c r="C48">
+        <v>34.07</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>-0.33200000000000002</v>
+      </c>
+      <c r="C49">
+        <v>34.073</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>-0.3</v>
+      </c>
+      <c r="C50">
+        <v>34.076999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>-0.23899999999999999</v>
+      </c>
+      <c r="C51">
+        <v>34.087000000000003</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>-0.158</v>
+      </c>
+      <c r="C52">
+        <v>34.103000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>-0.106</v>
+      </c>
+      <c r="C53">
+        <v>34.128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>-0.13700000000000001</v>
+      </c>
+      <c r="C54">
+        <v>34.121000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>-0.128</v>
+      </c>
+      <c r="C55">
+        <v>34.130000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>-5.7000000000000002E-2</v>
+      </c>
+      <c r="C56">
+        <v>34.158000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>53</v>
+      </c>
+      <c r="B57">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="C57">
+        <v>34.170999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>54</v>
+      </c>
+      <c r="B58">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C58">
+        <v>34.171999999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>55</v>
+      </c>
+      <c r="B59">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C59">
+        <v>34.168999999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C60">
+        <v>34.171999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>57</v>
+      </c>
+      <c r="B61">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C61">
+        <v>34.167999999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>0.06</v>
+      </c>
+      <c r="C62">
+        <v>34.183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>59</v>
+      </c>
+      <c r="B63">
+        <v>0.1</v>
+      </c>
+      <c r="C63">
+        <v>34.192</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <v>0.115</v>
+      </c>
+      <c r="C64">
+        <v>34.192999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>61</v>
+      </c>
+      <c r="B65">
+        <v>0.123</v>
+      </c>
+      <c r="C65">
+        <v>34.195</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>62</v>
+      </c>
+      <c r="B66">
+        <v>0.127</v>
+      </c>
+      <c r="C66">
+        <v>34.195999999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>63</v>
+      </c>
+      <c r="B67">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C67">
+        <v>34.198999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="C68">
+        <v>34.198999999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>65</v>
+      </c>
+      <c r="B69">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="C69">
+        <v>34.203000000000003</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>66</v>
+      </c>
+      <c r="B70">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C70">
+        <v>34.204000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>67</v>
+      </c>
+      <c r="B71">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="C71">
+        <v>34.203000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D56"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="59.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1.024</v>
+      </c>
+      <c r="C5">
+        <v>33.433999999999997</v>
+      </c>
+      <c r="D5">
+        <f>B5-$B$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="C6">
+        <v>33.421999999999997</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:D27" si="0">B6-$B$5</f>
+        <v>-4.3000000000000038E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="C7">
+        <v>33.427999999999997</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-0.123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="C8">
+        <v>33.433999999999997</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-0.18100000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="C9">
+        <v>33.442999999999998</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-0.21100000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="C10">
+        <v>33.451000000000001</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-0.22599999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="C11">
+        <v>33.459000000000003</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-0.22899999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="C12">
+        <v>33.466000000000001</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-0.22899999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="C13">
+        <v>33.478000000000002</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-0.22899999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>0.79900000000000004</v>
+      </c>
+      <c r="C14">
+        <v>33.491</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-0.22499999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="C15">
+        <v>33.497</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-0.21799999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="C16">
+        <v>33.502000000000002</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-0.20500000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="C17">
+        <v>33.517000000000003</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-0.18500000000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="C18">
+        <v>33.527999999999999</v>
+      </c>
+      <c r="D18">
+        <f>B18-$B$5</f>
+        <v>-0.17900000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="C19">
+        <v>33.54</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-0.19300000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="C20">
+        <v>33.555</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>-0.22099999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="C21">
+        <v>33.575000000000003</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-0.25700000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="C22">
+        <v>33.604999999999997</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-0.31200000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="C23">
+        <v>33.642000000000003</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>-0.38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>0.59099999999999997</v>
+      </c>
+      <c r="C24">
+        <v>33.673000000000002</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-0.43300000000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="C25">
+        <v>33.692</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>-0.45700000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="C26">
+        <v>33.706000000000003</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-0.47899999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>0.504</v>
+      </c>
+      <c r="C27">
+        <v>33.725999999999999</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>-0.52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="C28">
+        <v>33.747</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="C29">
+        <v>33.761000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>0.40799999999999997</v>
+      </c>
+      <c r="C30">
+        <v>33.768999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="C31">
+        <v>33.776000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>0.377</v>
+      </c>
+      <c r="C32">
+        <v>33.783000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>0.36</v>
+      </c>
+      <c r="C33">
+        <v>33.790999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="C34">
+        <v>33.802</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>0.314</v>
+      </c>
+      <c r="C35">
+        <v>33.814</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="C36">
+        <v>33.822000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="C37">
+        <v>33.825000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="C38">
+        <v>33.828000000000003</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="C39">
+        <v>33.834000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>0.248</v>
+      </c>
+      <c r="C40">
+        <v>33.847000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>0.216</v>
+      </c>
+      <c r="C41">
+        <v>33.866</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>0.187</v>
+      </c>
+      <c r="C42">
+        <v>33.886000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="C43">
+        <v>33.905000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="C44">
+        <v>33.920999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="C45">
+        <v>33.927999999999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>42</v>
+      </c>
+      <c r="B46">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C46">
+        <v>33.930999999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>43</v>
+      </c>
+      <c r="B47">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="C47">
+        <v>33.932000000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>44</v>
+      </c>
+      <c r="B48">
+        <v>0.126</v>
+      </c>
+      <c r="C48">
+        <v>33.936999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>45</v>
+      </c>
+      <c r="B49">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="C49">
+        <v>33.947000000000003</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>46</v>
+      </c>
+      <c r="B50">
+        <v>0.114</v>
+      </c>
+      <c r="C50">
+        <v>33.954999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>47</v>
+      </c>
+      <c r="B51">
+        <v>0.11</v>
+      </c>
+      <c r="C51">
+        <v>33.963999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>48</v>
+      </c>
+      <c r="B52">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="C52">
+        <v>33.972000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>49</v>
+      </c>
+      <c r="B53">
+        <v>9.4E-2</v>
+      </c>
+      <c r="C53">
+        <v>33.981000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>50</v>
+      </c>
+      <c r="B54">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="C54">
+        <v>33.994</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>51</v>
+      </c>
+      <c r="B55">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="C55">
+        <v>34.011000000000003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>52</v>
+      </c>
+      <c r="B56">
+        <v>0.06</v>
+      </c>
+      <c r="C56">
+        <v>34.024999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
@@ -1144,12 +2840,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1159,27 +2855,27 @@
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1189,8 +2885,12 @@
       <c r="C5">
         <v>-999</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f>B5-$B$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1200,8 +2900,12 @@
       <c r="C6">
         <v>33.941000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" ref="D6:D14" si="0">B6-$B$5</f>
+        <v>-0.15100000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1211,8 +2915,12 @@
       <c r="C7">
         <v>33.901000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-0.24100000000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1222,8 +2930,12 @@
       <c r="C8">
         <v>33.893000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-0.29900000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1233,8 +2945,12 @@
       <c r="C9">
         <v>33.896000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-0.34300000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1244,8 +2960,12 @@
       <c r="C10">
         <v>33.902999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-0.38000000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1255,8 +2975,12 @@
       <c r="C11">
         <v>33.911999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-0.41800000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1266,8 +2990,12 @@
       <c r="C12">
         <v>33.923000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-0.45200000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1277,8 +3005,12 @@
       <c r="C13">
         <v>33.933999999999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-0.48300000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1288,8 +3020,12 @@
       <c r="C14">
         <v>33.950000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-0.51900000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1300,7 +3036,7 @@
         <v>33.966000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1756,12 +3492,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1771,27 +3507,27 @@
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1801,8 +3537,12 @@
       <c r="C5">
         <v>33.869999999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f>B5-$B$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1812,8 +3552,12 @@
       <c r="C6">
         <v>33.871000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" ref="D6:D19" si="0">B6-$B$5</f>
+        <v>-7.5999999999999984E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1823,8 +3567,12 @@
       <c r="C7">
         <v>33.878999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1834,8 +3582,12 @@
       <c r="C8">
         <v>33.889000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-0.11899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1845,8 +3597,12 @@
       <c r="C9">
         <v>33.899000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-0.14499999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1856,8 +3612,12 @@
       <c r="C10">
         <v>33.902999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-0.16799999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1867,8 +3627,12 @@
       <c r="C11">
         <v>33.911000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-0.19700000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1878,8 +3642,12 @@
       <c r="C12">
         <v>33.914000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1889,8 +3657,12 @@
       <c r="C13">
         <v>33.92</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-0.27499999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1900,8 +3672,12 @@
       <c r="C14">
         <v>33.926000000000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-0.308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1911,8 +3687,12 @@
       <c r="C15">
         <v>33.932000000000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-0.33499999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1922,8 +3702,12 @@
       <c r="C16">
         <v>33.948</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1933,8 +3717,12 @@
       <c r="C17">
         <v>33.966000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-0.40100000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1944,8 +3732,12 @@
       <c r="C18">
         <v>33.978000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-0.46199999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1955,8 +3747,12 @@
       <c r="C19">
         <v>33.991999999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-0.52700000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1967,7 +3763,7 @@
         <v>34.008000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1978,7 +3774,7 @@
         <v>34.021000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1989,7 +3785,7 @@
         <v>34.024999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2000,7 +3796,7 @@
         <v>34.029000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2011,7 +3807,7 @@
         <v>34.034999999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2022,7 +3818,7 @@
         <v>34.045000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2033,7 +3829,7 @@
         <v>34.054000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>23</v>
       </c>
@@ -2044,7 +3840,7 @@
         <v>34.06</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>24</v>
       </c>
@@ -2055,7 +3851,7 @@
         <v>34.078000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2066,7 +3862,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2077,7 +3873,7 @@
         <v>34.103000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>27</v>
       </c>
@@ -2088,7 +3884,7 @@
         <v>34.11</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>28</v>
       </c>
@@ -2104,12 +3900,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2119,27 +3915,27 @@
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2149,8 +3945,12 @@
       <c r="C5">
         <v>32.383000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f>B5-$B$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2160,8 +3960,12 @@
       <c r="C6">
         <v>32.718000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" ref="D6:D17" si="0">B6-$B$5</f>
+        <v>0.21599999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2171,8 +3975,12 @@
       <c r="C7">
         <v>33.012</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.42400000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2182,8 +3990,12 @@
       <c r="C8">
         <v>33.200000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.54900000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2193,8 +4005,12 @@
       <c r="C9">
         <v>33.350999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.60799999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2204,8 +4020,12 @@
       <c r="C10">
         <v>33.450000000000003</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.63700000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2215,8 +4035,12 @@
       <c r="C11">
         <v>33.545999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.71599999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2226,8 +4050,12 @@
       <c r="C12">
         <v>33.618000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2237,8 +4065,12 @@
       <c r="C13">
         <v>33.637</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.72099999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2248,8 +4080,12 @@
       <c r="C14">
         <v>33.668999999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.70099999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2259,8 +4095,12 @@
       <c r="C15">
         <v>33.712000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0.70399999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2270,8 +4110,12 @@
       <c r="C16">
         <v>33.776000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -2281,8 +4125,12 @@
       <c r="C17">
         <v>33.835999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
@@ -2293,7 +4141,7 @@
         <v>33.877000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
@@ -2304,7 +4152,7 @@
         <v>33.904000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2315,7 +4163,7 @@
         <v>33.935000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2326,7 +4174,7 @@
         <v>33.963999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2337,7 +4185,7 @@
         <v>33.994</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2348,7 +4196,7 @@
         <v>34.014000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2359,7 +4207,7 @@
         <v>34.026000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2370,7 +4218,7 @@
         <v>34.037999999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2381,7 +4229,7 @@
         <v>34.052</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>23</v>
       </c>
@@ -2392,7 +4240,7 @@
         <v>34.058999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>24</v>
       </c>
@@ -2403,7 +4251,7 @@
         <v>34.067999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2414,7 +4262,7 @@
         <v>34.082999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2425,7 +4273,7 @@
         <v>34.103000000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>27</v>
       </c>
@@ -2436,7 +4284,7 @@
         <v>34.113999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>28</v>
       </c>
@@ -2716,12 +4564,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2731,27 +4579,27 @@
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2761,8 +4609,12 @@
       <c r="C5">
         <v>32.814</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <f>B5-$B$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2772,8 +4624,12 @@
       <c r="C6">
         <v>33.095999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" ref="D6:D14" si="0">B6-$B$5</f>
+        <v>-8.4999999999999964E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2783,8 +4639,12 @@
       <c r="C7">
         <v>33.244999999999997</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-7.9999999999999849E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2794,8 +4654,12 @@
       <c r="C8">
         <v>33.389000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.4000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2805,8 +4669,12 @@
       <c r="C9">
         <v>33.482999999999997</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.10099999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2816,8 +4684,12 @@
       <c r="C10">
         <v>33.576999999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.22100000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2827,8 +4699,12 @@
       <c r="C11">
         <v>33.706000000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2838,8 +4714,12 @@
       <c r="C12">
         <v>33.808</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2849,8 +4729,12 @@
       <c r="C13">
         <v>33.890999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.63400000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2860,8 +4744,12 @@
       <c r="C14">
         <v>33.953000000000003</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.72700000000000009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2872,7 +4760,7 @@
         <v>33.993000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3338,4 +5226,106 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" zoomScalePageLayoutView="126" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1">
+        <v>41620</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1">
+        <v>41632</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1">
+        <v>41635</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="1">
+        <v>41641</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1">
+        <v>41635</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="1">
+        <v>41641</v>
+      </c>
+      <c r="C10">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>